<commit_message>
updated variables names & added historic page
</commit_message>
<xml_diff>
--- a/tables/reg_semanais.xlsx
+++ b/tables/reg_semanais.xlsx
@@ -16,10 +16,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -58,12 +55,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -429,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1:V11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,90 +446,95 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>interv_dia</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>pre_pas1</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>pre_pad1</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>pre_pas2</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>pre_pad2</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>pre_pas3</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>pre_pad3</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>pos_pas1</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>pos_pad1</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>pos_pas2</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>pos_pad2</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>pos_pas3</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>pos_pad3</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>pre_glic1</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>pre_glic2</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>pre_glic3</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>pos_glic1</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>pos_glic2</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>pos_glic3</t>
         </is>
@@ -545,20 +546,24 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Adeilda Alves Siqueira</t>
-        </is>
-      </c>
-      <c r="C2" s="2" t="n">
-        <v>44972</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0</v>
+          <t>Selecionar Nome Completo</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>28/02/23</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Relaxamento</t>
+        </is>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
@@ -573,10 +578,10 @@
         <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>140</v>
       </c>
       <c r="L2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M2" t="n">
         <v>0</v>
@@ -603,6 +608,9 @@
         <v>0</v>
       </c>
       <c r="U2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -612,26 +620,30 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Adeilda Alves Siqueira</t>
-        </is>
-      </c>
-      <c r="C3" s="2" t="n">
-        <v>44972</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0</v>
+          <t>Selecionar Nome Completo</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>01/03/23</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Hidro</t>
+        </is>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>130</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>125</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="I3" t="n">
         <v>0</v>
@@ -640,10 +652,10 @@
         <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>0</v>
+        <v>140</v>
       </c>
       <c r="L3" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M3" t="n">
         <v>0</v>
@@ -658,7 +670,7 @@
         <v>0</v>
       </c>
       <c r="Q3" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="R3" t="n">
         <v>0</v>
@@ -667,9 +679,604 @@
         <v>0</v>
       </c>
       <c r="T3" t="n">
-        <v>0</v>
+        <v>95</v>
       </c>
       <c r="U3" t="n">
+        <v>0</v>
+      </c>
+      <c r="V3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Selecionar Nome Completo</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>03/03/23</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Pilates</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>123</v>
+      </c>
+      <c r="F4" t="n">
+        <v>78</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>140</v>
+      </c>
+      <c r="L4" t="n">
+        <v>100</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0</v>
+      </c>
+      <c r="U4" t="n">
+        <v>0</v>
+      </c>
+      <c r="V4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Selecionar Nome Completo</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>31/03/23</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Relaxamento</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>123</v>
+      </c>
+      <c r="F5" t="n">
+        <v>78</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>140</v>
+      </c>
+      <c r="L5" t="n">
+        <v>100</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0</v>
+      </c>
+      <c r="U5" t="n">
+        <v>0</v>
+      </c>
+      <c r="V5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Selecionar Nome Completo</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>03/04/23</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Hidro</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>120</v>
+      </c>
+      <c r="F6" t="n">
+        <v>80</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="n">
+        <v>140</v>
+      </c>
+      <c r="L6" t="n">
+        <v>100</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>0</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0</v>
+      </c>
+      <c r="U6" t="n">
+        <v>0</v>
+      </c>
+      <c r="V6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Selecionar Nome Completo</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>05/05/23</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Pilates</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>130</v>
+      </c>
+      <c r="F7" t="n">
+        <v>90</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>140</v>
+      </c>
+      <c r="L7" t="n">
+        <v>100</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T7" t="n">
+        <v>0</v>
+      </c>
+      <c r="U7" t="n">
+        <v>0</v>
+      </c>
+      <c r="V7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Selecionar Nome Completo</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>08/05/23</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Não fez aula</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>120</v>
+      </c>
+      <c r="F8" t="n">
+        <v>90</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>90</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0</v>
+      </c>
+      <c r="P8" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>120</v>
+      </c>
+      <c r="R8" t="n">
+        <v>0</v>
+      </c>
+      <c r="S8" t="n">
+        <v>0</v>
+      </c>
+      <c r="T8" t="n">
+        <v>100</v>
+      </c>
+      <c r="U8" t="n">
+        <v>0</v>
+      </c>
+      <c r="V8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Amara Maria A. da Silva (Bolsa 100%)</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>08/05/23</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Hidro</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>100</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>90</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0</v>
+      </c>
+      <c r="P9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>0</v>
+      </c>
+      <c r="R9" t="n">
+        <v>0</v>
+      </c>
+      <c r="S9" t="n">
+        <v>0</v>
+      </c>
+      <c r="T9" t="n">
+        <v>0</v>
+      </c>
+      <c r="U9" t="n">
+        <v>0</v>
+      </c>
+      <c r="V9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Josefa Pereira Silva</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>08/05/23</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Hidro</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>101</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0</v>
+      </c>
+      <c r="P10" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>129</v>
+      </c>
+      <c r="R10" t="n">
+        <v>0</v>
+      </c>
+      <c r="S10" t="n">
+        <v>0</v>
+      </c>
+      <c r="T10" t="n">
+        <v>0</v>
+      </c>
+      <c r="U10" t="n">
+        <v>0</v>
+      </c>
+      <c r="V10" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Selecionar Nome Completo</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>09/05/23</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Pilates</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>120</v>
+      </c>
+      <c r="F11" t="n">
+        <v>123</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" t="n">
+        <v>90</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0</v>
+      </c>
+      <c r="P11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>0</v>
+      </c>
+      <c r="R11" t="n">
+        <v>0</v>
+      </c>
+      <c r="S11" t="n">
+        <v>0</v>
+      </c>
+      <c r="T11" t="n">
+        <v>0</v>
+      </c>
+      <c r="U11" t="n">
+        <v>0</v>
+      </c>
+      <c r="V11" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>